<commit_message>
collect all infos , quotes + Answering emails 22/12/2024
</commit_message>
<xml_diff>
--- a/BOM-Lab.xlsx
+++ b/BOM-Lab.xlsx
@@ -117,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -128,9 +128,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -140,12 +137,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -155,10 +146,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,7 +446,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,117 +471,118 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>